<commit_message>
Updated ocnbgchem for MIROC-ES2L.
</commit_message>
<xml_diff>
--- a/cmip6/models/miroc-es2l/cmip6_miroc_miroc-es2l_ocnbgchem.xlsx
+++ b/cmip6/models/miroc-es2l/cmip6_miroc_miroc-es2l_ocnbgchem.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d566ba9b8f1570b/仕事/ES-DOC/SharedForWriters/models/miroc-es2l/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="71" documentId="11_D4710AA95E59BCAC088416C93A9FCFC95EF5E6CE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9F2615B6-C830-40A9-BB20-AACB1CDC335D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,23 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Tracers" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="454">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -106,6 +123,21 @@
     <t>Role</t>
   </si>
   <si>
+    <t>WATANABE-MCH</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>YAMAMOTO-A</t>
+  </si>
+  <si>
+    <t>NOGUCHI-M</t>
+  </si>
+  <si>
+    <t>KAWAMIYA-M</t>
+  </si>
+  <si>
     <t>Citations</t>
   </si>
   <si>
@@ -118,12 +150,42 @@
     <t>Process</t>
   </si>
   <si>
+    <t>Leonard_1979</t>
+  </si>
+  <si>
+    <t>Key Properties</t>
+  </si>
+  <si>
+    <t>Leonard_1993</t>
+  </si>
+  <si>
+    <t>Leonard_1994</t>
+  </si>
+  <si>
+    <t>Kobayashi_2018</t>
+  </si>
+  <si>
+    <t>Simo_2002</t>
+  </si>
+  <si>
+    <t>Aranami_2004</t>
+  </si>
+  <si>
+    <t>Wanninkhof_2014</t>
+  </si>
+  <si>
+    <t>Orr_2017</t>
+  </si>
+  <si>
+    <t>Moore_2008</t>
+  </si>
+  <si>
+    <t>Tagliabue_2010</t>
+  </si>
+  <si>
     <t>1.1.1</t>
   </si>
   <si>
-    <t>Key Properties</t>
-  </si>
-  <si>
     <t>Ocean Biogeochemistry key properties</t>
   </si>
   <si>
@@ -271,6 +333,9 @@
     <t>cmip6.ocnbgchem.key_properties.diagnostic_variables</t>
   </si>
   <si>
+    <t>DMS</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.1.9 </t>
   </si>
   <si>
@@ -281,6 +346,9 @@
   </si>
   <si>
     <t>cmip6.ocnbgchem.key_properties.damping</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>1.1.2</t>
@@ -1333,12 +1401,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1435,6 +1503,13 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1526,15 +1601,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1576,7 +1659,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1608,9 +1691,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1642,6 +1743,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1817,24 +1936,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.7265625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="32.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1842,7 +1961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1850,7 +1969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1858,7 +1977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1866,7 +1985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1874,12 +1993,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1887,7 +2006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="17.5">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1895,7 +2014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1903,7 +2022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1911,41 +2030,44 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1956,7 +2078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1980,400 +2102,511 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="9" t="s">
+    <row r="9" spans="1:2" ht="17.5">
+      <c r="A9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+    <row r="10" spans="1:2" ht="17.5">
+      <c r="A10" s="11" t="s">
         <v>31</v>
       </c>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.5">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17.5">
+      <c r="A12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18">
+      <c r="A15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="B19" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17.5">
+      <c r="A20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17.5">
+      <c r="A21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17.5">
+      <c r="A22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17.5">
+      <c r="A23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17.5">
+      <c r="A24" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17.5">
+      <c r="A25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17.5">
+      <c r="A26" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17.5">
+      <c r="A27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17.5">
+      <c r="A28" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17.5">
+      <c r="A29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B29" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>"Top Level,Key Properties,Tracers"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B12" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
-      <formula1>"Top Level,Key Properties,Tracers"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD235"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AD235"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="41.25" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="204" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="24" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AA20" s="6" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="24" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="AA24" s="6" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="AB24" s="6" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="AC24" s="6" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="24" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="24" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="24" customHeight="1">
       <c r="B28" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="24" customHeight="1">
       <c r="B29" s="11" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="24" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="B33" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="39" customHeight="1">
       <c r="B34" s="11" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="24" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
       <c r="B38" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
       <c r="A42" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="B43" s="11"/>
+      <c r="B43" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="B47" s="13" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="24" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="24" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="24" customHeight="1">
       <c r="B51" s="11" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="AA51" s="6" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="AB51" s="6" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="24" customHeight="1">
       <c r="A54" s="14" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="24" customHeight="1">
@@ -2381,64 +2614,64 @@
     </row>
     <row r="58" spans="1:28" ht="24" customHeight="1">
       <c r="A58" s="12" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="24" customHeight="1">
       <c r="B59" s="13" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="24" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="24" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="24" customHeight="1">
       <c r="B63" s="11" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="AA63" s="6" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="AB63" s="6" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:28" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:28" ht="24" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="24" customHeight="1">
@@ -2446,271 +2679,273 @@
     </row>
     <row r="70" spans="1:28" ht="24" customHeight="1">
       <c r="A70" s="12" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="24" customHeight="1">
       <c r="B71" s="13" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="24" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="24" customHeight="1">
       <c r="B75" s="11" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="AA75" s="6" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="AB75" s="6" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="24" customHeight="1">
       <c r="A77" s="9" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="24" customHeight="1">
       <c r="A78" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="24" customHeight="1">
       <c r="B79" s="11" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="AA79" s="6" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="AB79" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:29" ht="24" customHeight="1">
       <c r="A81" s="9" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:29" ht="24" customHeight="1">
       <c r="A82" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:29" ht="24" customHeight="1">
       <c r="B83" s="8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="178" customHeight="1">
       <c r="B84" s="11" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
     </row>
     <row r="87" spans="1:29" ht="24" customHeight="1">
       <c r="A87" s="12" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:29" ht="24" customHeight="1">
       <c r="B88" s="13" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:29" ht="24" customHeight="1">
       <c r="A90" s="9" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:29" ht="24" customHeight="1">
       <c r="A91" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:29" ht="24" customHeight="1">
       <c r="B92" s="11" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="AA92" s="6" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="AB92" s="6" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="AC92" s="6" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:29" ht="24" customHeight="1">
       <c r="A94" s="9" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:29" ht="24" customHeight="1">
       <c r="A95" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:29" ht="24" customHeight="1">
       <c r="B96" s="11" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="AA96" s="6" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="AB96" s="6" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="AC96" s="6" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
       <c r="A98" s="9" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="A99" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
       <c r="B100" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
       <c r="B101" s="11" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
       <c r="A104" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
       <c r="B105" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
-      <c r="B106" s="11"/>
+      <c r="B106" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
       <c r="A109" s="12" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
       <c r="B110" s="13" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
       <c r="A112" s="9" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="24" customHeight="1">
       <c r="A113" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="114" spans="1:28" ht="24" customHeight="1">
@@ -2720,51 +2955,51 @@
     </row>
     <row r="116" spans="1:28" ht="24" customHeight="1">
       <c r="A116" s="9" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="24" customHeight="1">
       <c r="A117" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="24" customHeight="1">
       <c r="B118" s="11" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="AA118" s="6" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="AB118" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="24" customHeight="1">
       <c r="A120" s="9" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="24" customHeight="1">
       <c r="A121" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="24" customHeight="1">
@@ -2774,51 +3009,51 @@
     </row>
     <row r="124" spans="1:28" ht="24" customHeight="1">
       <c r="A124" s="9" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
     </row>
     <row r="125" spans="1:28" ht="24" customHeight="1">
       <c r="A125" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
     </row>
     <row r="126" spans="1:28" ht="24" customHeight="1">
       <c r="B126" s="11" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="AA126" s="6" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="AB126" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="128" spans="1:28" ht="24" customHeight="1">
       <c r="A128" s="9" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
       <c r="A129" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="24" customHeight="1">
@@ -2828,45 +3063,45 @@
     </row>
     <row r="132" spans="1:3" ht="24" customHeight="1">
       <c r="A132" s="9" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="24" customHeight="1">
       <c r="A133" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
       <c r="B134" s="11" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="24" customHeight="1">
       <c r="A136" s="9" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="24" customHeight="1">
       <c r="A137" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="24" customHeight="1">
@@ -2876,43 +3111,45 @@
     </row>
     <row r="140" spans="1:3" ht="24" customHeight="1">
       <c r="A140" s="9" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="24" customHeight="1">
       <c r="A141" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="24" customHeight="1">
-      <c r="B142" s="11"/>
+      <c r="B142" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
       <c r="A144" s="9" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="24" customHeight="1">
       <c r="A145" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="24" customHeight="1">
@@ -2922,45 +3159,45 @@
     </row>
     <row r="148" spans="1:3" ht="24" customHeight="1">
       <c r="A148" s="9" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
       <c r="A149" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="24" customHeight="1">
       <c r="B150" s="11" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="24" customHeight="1">
       <c r="A152" s="9" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="24" customHeight="1">
       <c r="A153" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1">
@@ -2970,43 +3207,45 @@
     </row>
     <row r="156" spans="1:3" ht="24" customHeight="1">
       <c r="A156" s="9" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="24" customHeight="1">
       <c r="A157" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="24" customHeight="1">
-      <c r="B158" s="11"/>
+      <c r="B158" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
       <c r="A160" s="9" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="24" customHeight="1">
       <c r="A161" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="24" customHeight="1">
@@ -3016,43 +3255,45 @@
     </row>
     <row r="164" spans="1:3" ht="24" customHeight="1">
       <c r="A164" s="9" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="24" customHeight="1">
       <c r="A165" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="24" customHeight="1">
-      <c r="B166" s="11"/>
+      <c r="B166" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1">
       <c r="A168" s="9" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="24" customHeight="1">
       <c r="A169" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="24" customHeight="1">
@@ -3062,43 +3303,45 @@
     </row>
     <row r="172" spans="1:3" ht="24" customHeight="1">
       <c r="A172" s="9" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1">
       <c r="A173" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="24" customHeight="1">
-      <c r="B174" s="11"/>
+      <c r="B174" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="176" spans="1:3" ht="24" customHeight="1">
       <c r="A176" s="9" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="24" customHeight="1">
       <c r="A177" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1">
@@ -3108,43 +3351,45 @@
     </row>
     <row r="180" spans="1:3" ht="24" customHeight="1">
       <c r="A180" s="9" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="24" customHeight="1">
       <c r="A181" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="24" customHeight="1">
-      <c r="B182" s="11"/>
+      <c r="B182" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="184" spans="1:3" ht="24" customHeight="1">
       <c r="A184" s="9" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="24" customHeight="1">
       <c r="A185" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="24" customHeight="1">
@@ -3154,144 +3399,148 @@
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1">
       <c r="A188" s="9" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="24" customHeight="1">
       <c r="A189" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="24" customHeight="1">
-      <c r="B190" s="11"/>
+      <c r="B190" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="192" spans="1:3" ht="24" customHeight="1">
       <c r="A192" s="9" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
     </row>
     <row r="193" spans="1:29" ht="24" customHeight="1">
       <c r="A193" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B193" s="10" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
     </row>
     <row r="194" spans="1:29" ht="24" customHeight="1">
-      <c r="B194" s="11"/>
+      <c r="B194" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="197" spans="1:29" ht="24" customHeight="1">
       <c r="A197" s="12" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="198" spans="1:29" ht="24" customHeight="1">
       <c r="B198" s="13" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
     </row>
     <row r="200" spans="1:29" ht="24" customHeight="1">
       <c r="A200" s="9" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="201" spans="1:29" ht="24" customHeight="1">
       <c r="A201" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B201" s="10" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
     </row>
     <row r="202" spans="1:29" ht="24" customHeight="1">
       <c r="B202" s="11" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="AA202" s="6" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="AB202" s="6" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
     </row>
     <row r="204" spans="1:29" ht="24" customHeight="1">
       <c r="A204" s="9" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
     </row>
     <row r="205" spans="1:29" ht="24" customHeight="1">
       <c r="A205" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B205" s="10" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
     </row>
     <row r="206" spans="1:29" ht="24" customHeight="1">
       <c r="B206" s="11"/>
       <c r="AA206" s="6" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="AB206" s="6" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="AC206" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="208" spans="1:29" ht="24" customHeight="1">
       <c r="A208" s="9" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
       <c r="A209" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="24" customHeight="1">
       <c r="B210" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="24" customHeight="1">
@@ -3299,200 +3548,150 @@
     </row>
     <row r="214" spans="1:3" ht="24" customHeight="1">
       <c r="A214" s="12" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="24" customHeight="1">
       <c r="B215" s="13" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="24" customHeight="1">
       <c r="A217" s="9" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1">
       <c r="A218" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="24" customHeight="1">
       <c r="B219" s="8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="178" customHeight="1">
       <c r="B220" s="11" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="24" customHeight="1">
       <c r="A222" s="9" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="24" customHeight="1">
       <c r="A223" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="24" customHeight="1">
       <c r="B224" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="24" customHeight="1">
-      <c r="B225" s="11"/>
+      <c r="B225" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="227" spans="1:3" ht="24" customHeight="1">
       <c r="A227" s="9" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="24" customHeight="1">
       <c r="A228" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B228" s="10" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="24" customHeight="1">
       <c r="B229" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="24" customHeight="1">
-      <c r="B230" s="11"/>
+      <c r="B230" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="232" spans="1:3" ht="24" customHeight="1">
       <c r="A232" s="9" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="24" customHeight="1">
       <c r="A233" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B233" s="10" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="C233" s="10" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="24" customHeight="1">
       <c r="B234" s="8" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="24" customHeight="1">
-      <c r="B235" s="11"/>
+      <c r="B235" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="24">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA20:AD20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B206 B96 B92" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AA24:AC24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B202 B126 B118 B79 B75 B63" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>AA51:AB51</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 B67" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
-      <formula1>AA63:AB63</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>AA75:AB75</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
-      <formula1>AA79:AB79</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92">
-      <formula1>AA92:AC92</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B96">
-      <formula1>AA96:AC96</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114 B186 B178 B170 B162 B154 B146 B138 B130 B122" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B118">
-      <formula1>AA118:AB118</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B126">
-      <formula1>AA126:AB126</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B130">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B138">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B146">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B154">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B162">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B170">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B178">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B186">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B202">
-      <formula1>AA202:AB202</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B206">
-      <formula1>AA206:AC206</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3500,102 +3699,104 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AE132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>288</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
@@ -3605,21 +3806,21 @@
     </row>
     <row r="17" spans="1:31" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="24" customHeight="1">
@@ -3629,81 +3830,81 @@
     </row>
     <row r="20" spans="1:31" ht="24" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="AA20" s="6" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="AE20" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="24" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="AA21" s="6" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="AE21" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="24" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="AA22" s="6" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="AB22" s="6" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="AC22" s="6" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="AD22" s="6" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="AE22" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="24" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="24" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="24" customHeight="1">
@@ -3713,35 +3914,35 @@
     </row>
     <row r="27" spans="1:31" ht="24" customHeight="1">
       <c r="B27" s="11" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="AA27" s="6" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="AB27" s="6" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="AC27" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="24" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="24" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:31" ht="24" customHeight="1">
@@ -3751,158 +3952,162 @@
     </row>
     <row r="32" spans="1:31" ht="24" customHeight="1">
       <c r="B32" s="11" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="AA32" s="6" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="AB32" s="6" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="AC32" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="24" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="AA33" s="6" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="AB33" s="6" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="AC33" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="24" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>321</v>
+        <v>338</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="24" customHeight="1">
       <c r="B37" s="13" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="24" customHeight="1">
       <c r="A40" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="43" spans="1:29" ht="24" customHeight="1">
       <c r="A43" s="9" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>329</v>
+        <v>346</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="24" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="24" customHeight="1">
-      <c r="B45" s="11"/>
+      <c r="B45" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="48" spans="1:29" ht="24" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
     </row>
     <row r="49" spans="1:31" ht="24" customHeight="1">
       <c r="B49" s="13" t="s">
-        <v>334</v>
+        <v>351</v>
       </c>
     </row>
     <row r="51" spans="1:31" ht="24" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:31" ht="24" customHeight="1">
       <c r="A52" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>337</v>
+        <v>354</v>
       </c>
     </row>
     <row r="53" spans="1:31" ht="24" customHeight="1">
       <c r="B53" s="11" t="s">
-        <v>338</v>
+        <v>355</v>
       </c>
       <c r="AA53" s="6" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="AB53" s="6" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="AC53" s="6" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="AD53" s="6" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="AE53" s="6" t="s">
-        <v>338</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:31" ht="24" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>344</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:31" ht="24" customHeight="1">
       <c r="A56" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>346</v>
+        <v>363</v>
       </c>
     </row>
     <row r="57" spans="1:31" ht="24" customHeight="1">
@@ -3912,55 +4117,55 @@
     </row>
     <row r="58" spans="1:31" ht="24" customHeight="1">
       <c r="B58" s="11" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="AA58" s="6" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="AB58" s="6" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="AC58" s="6" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="AD58" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:31" ht="24" customHeight="1">
       <c r="B59" s="11" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="AA59" s="6" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="AB59" s="6" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="AC59" s="6" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="AD59" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:31" ht="24" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>350</v>
+        <v>367</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>351</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" spans="1:31" ht="24" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:31" ht="24" customHeight="1">
@@ -3971,84 +4176,84 @@
     <row r="64" spans="1:31" ht="24" customHeight="1">
       <c r="B64" s="11"/>
       <c r="AA64" s="6" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
       <c r="AB64" s="6" t="s">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="AC64" s="6" t="s">
-        <v>356</v>
+        <v>373</v>
       </c>
       <c r="AD64" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:30" ht="24" customHeight="1">
       <c r="A67" s="12" t="s">
-        <v>357</v>
+        <v>374</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>358</v>
+        <v>375</v>
       </c>
     </row>
     <row r="68" spans="1:30" ht="24" customHeight="1">
       <c r="B68" s="13" t="s">
-        <v>359</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" spans="1:30" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:30" ht="24" customHeight="1">
       <c r="A71" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>361</v>
+        <v>378</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>362</v>
+        <v>379</v>
       </c>
     </row>
     <row r="72" spans="1:30" ht="24" customHeight="1">
       <c r="B72" s="11" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="AA72" s="6" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="AB72" s="6" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="AC72" s="6" t="s">
-        <v>363</v>
+        <v>380</v>
       </c>
       <c r="AD72" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:30" ht="24" customHeight="1">
       <c r="A74" s="9" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>351</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:30" ht="24" customHeight="1">
       <c r="A75" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>365</v>
+        <v>382</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>366</v>
+        <v>383</v>
       </c>
     </row>
     <row r="76" spans="1:30" ht="24" customHeight="1">
@@ -4059,45 +4264,45 @@
     <row r="77" spans="1:30" ht="24" customHeight="1">
       <c r="B77" s="11"/>
       <c r="AA77" s="6" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="AB77" s="6" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
       <c r="AC77" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:30" ht="24" customHeight="1">
       <c r="A80" s="12" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
     </row>
     <row r="81" spans="1:31" ht="24" customHeight="1">
       <c r="B81" s="13" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
     </row>
     <row r="83" spans="1:31" ht="24" customHeight="1">
       <c r="A83" s="9" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
     </row>
     <row r="84" spans="1:31" ht="24" customHeight="1">
       <c r="A84" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>374</v>
+        <v>391</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
     </row>
     <row r="85" spans="1:31" ht="24" customHeight="1">
@@ -4107,71 +4312,73 @@
     </row>
     <row r="87" spans="1:31" ht="24" customHeight="1">
       <c r="A87" s="9" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>377</v>
+        <v>394</v>
       </c>
     </row>
     <row r="88" spans="1:31" ht="24" customHeight="1">
       <c r="A88" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
     </row>
     <row r="89" spans="1:31" ht="24" customHeight="1">
-      <c r="B89" s="11"/>
+      <c r="B89" s="11" t="s">
+        <v>356</v>
+      </c>
       <c r="AA89" s="6" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="AB89" s="6" t="s">
-        <v>380</v>
+        <v>397</v>
       </c>
       <c r="AC89" s="6" t="s">
-        <v>381</v>
+        <v>398</v>
       </c>
       <c r="AD89" s="6" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
       <c r="AE89" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:31" ht="24" customHeight="1">
       <c r="A92" s="12" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:31" ht="24" customHeight="1">
       <c r="B93" s="13" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
     </row>
     <row r="95" spans="1:31" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>386</v>
+        <v>403</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:31" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>388</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" spans="1:31" ht="24" customHeight="1">
@@ -4181,41 +4388,41 @@
     </row>
     <row r="98" spans="1:31" ht="24" customHeight="1">
       <c r="B98" s="11" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="AA98" s="6" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="AB98" s="6" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="AC98" s="6" t="s">
-        <v>391</v>
+        <v>408</v>
       </c>
       <c r="AD98" s="6" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="AE98" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:31" ht="24" customHeight="1">
       <c r="A100" s="9" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>394</v>
+        <v>411</v>
       </c>
     </row>
     <row r="101" spans="1:31" ht="24" customHeight="1">
       <c r="A101" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>395</v>
+        <v>412</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>396</v>
+        <v>413</v>
       </c>
     </row>
     <row r="102" spans="1:31" ht="24" customHeight="1">
@@ -4225,74 +4432,74 @@
     </row>
     <row r="103" spans="1:31" ht="24" customHeight="1">
       <c r="B103" s="11" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="AA103" s="6" t="s">
-        <v>397</v>
+        <v>414</v>
       </c>
       <c r="AB103" s="6" t="s">
-        <v>398</v>
+        <v>415</v>
       </c>
       <c r="AC103" s="6" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="AD103" s="6" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
       <c r="AE103" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="105" spans="1:31" ht="24" customHeight="1">
       <c r="A105" s="9" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
     </row>
     <row r="106" spans="1:31" ht="24" customHeight="1">
       <c r="A106" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>403</v>
+        <v>420</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>404</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107" spans="1:31" ht="24" customHeight="1">
       <c r="B107" s="11" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="AA107" s="6" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="AB107" s="6" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="AC107" s="6" t="s">
-        <v>407</v>
+        <v>424</v>
       </c>
     </row>
     <row r="109" spans="1:31" ht="24" customHeight="1">
       <c r="A109" s="9" t="s">
-        <v>408</v>
+        <v>425</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
     </row>
     <row r="110" spans="1:31" ht="24" customHeight="1">
       <c r="A110" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>411</v>
+        <v>428</v>
       </c>
     </row>
     <row r="111" spans="1:31" ht="24" customHeight="1">
@@ -4300,70 +4507,70 @@
     </row>
     <row r="113" spans="1:30" ht="24" customHeight="1">
       <c r="A113" s="9" t="s">
-        <v>412</v>
+        <v>429</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>413</v>
+        <v>430</v>
       </c>
     </row>
     <row r="114" spans="1:30" ht="24" customHeight="1">
       <c r="A114" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
     </row>
     <row r="115" spans="1:30" ht="24" customHeight="1">
       <c r="B115" s="11" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="AA115" s="6" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="AB115" s="6" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="AC115" s="6" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="AD115" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="118" spans="1:30" ht="24" customHeight="1">
       <c r="A118" s="12" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>420</v>
+        <v>437</v>
       </c>
     </row>
     <row r="119" spans="1:30" ht="24" customHeight="1">
       <c r="B119" s="13" t="s">
-        <v>421</v>
+        <v>438</v>
       </c>
     </row>
     <row r="121" spans="1:30" ht="24" customHeight="1">
       <c r="A121" s="9" t="s">
-        <v>422</v>
+        <v>439</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>423</v>
+        <v>440</v>
       </c>
     </row>
     <row r="122" spans="1:30" ht="24" customHeight="1">
       <c r="A122" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>424</v>
+        <v>441</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>425</v>
+        <v>442</v>
       </c>
     </row>
     <row r="123" spans="1:30" ht="24" customHeight="1">
@@ -4374,29 +4581,29 @@
     <row r="124" spans="1:30" ht="24" customHeight="1">
       <c r="B124" s="11"/>
       <c r="AA124" s="6" t="s">
-        <v>426</v>
+        <v>443</v>
       </c>
       <c r="AB124" s="6" t="s">
-        <v>427</v>
+        <v>444</v>
       </c>
     </row>
     <row r="126" spans="1:30" ht="24" customHeight="1">
       <c r="A126" s="9" t="s">
-        <v>428</v>
+        <v>445</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>429</v>
+        <v>446</v>
       </c>
     </row>
     <row r="127" spans="1:30" ht="24" customHeight="1">
       <c r="A127" s="14" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B127" s="10" t="s">
-        <v>430</v>
+        <v>447</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>431</v>
+        <v>448</v>
       </c>
     </row>
     <row r="128" spans="1:30" ht="24" customHeight="1">
@@ -4406,99 +4613,51 @@
     </row>
     <row r="130" spans="1:28" ht="24" customHeight="1">
       <c r="A130" s="9" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
     </row>
     <row r="131" spans="1:28" ht="24" customHeight="1">
       <c r="A131" s="14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
       <c r="C131" s="10" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
     </row>
     <row r="132" spans="1:28" ht="24" customHeight="1">
-      <c r="B132" s="11"/>
+      <c r="B132" s="11" t="s">
+        <v>409</v>
+      </c>
       <c r="AA132" s="6" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="AB132" s="6" t="s">
-        <v>436</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="22">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B128 B85" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B103 B98 B89 B53 B20:B22" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>AA20:AE20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
-      <formula1>AA21:AE21</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
-      <formula1>AA22:AE22</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27 B107 B77 B32:B33" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>AA27:AC27</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
-      <formula1>AA32:AC32</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
-      <formula1>AA33:AC33</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53">
-      <formula1>AA53:AE53</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B115 B72 B64 B58:B59" xr:uid="{00000000-0002-0000-0300-000008000000}">
       <formula1>AA58:AD58</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
-      <formula1>AA59:AD59</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
-      <formula1>AA64:AD64</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
-      <formula1>AA72:AD72</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
-      <formula1>AA77:AC77</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B85">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
-      <formula1>AA89:AE89</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B98">
-      <formula1>AA98:AE98</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B103">
-      <formula1>AA103:AE103</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B107">
-      <formula1>AA107:AC107</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B115">
-      <formula1>AA115:AD115</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B124">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B124 B132" xr:uid="{00000000-0002-0000-0300-000013000000}">
       <formula1>AA124:AB124</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B128">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B132">
-      <formula1>AA132:AB132</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>